<commit_message>
updated statslibrary and formula sheet
</commit_message>
<xml_diff>
--- a/Project 1/Documents/Binomial&Geometric.xlsx
+++ b/Project 1/Documents/Binomial&Geometric.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rance\OneDrive\Documents\My Files\Other\College Class Materials\ThirdYearSpring\Probability and Applied Statistics\Projects\Project 1\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91D5D2A9-3A9D-4E76-A326-A23A862D2444}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04600334-DC63-4867-97B2-D376CF8A9213}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{D86DE10C-8526-4510-AA9E-43DF728B3974}"/>
   </bookViews>
@@ -155,11 +155,11 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Problem</a:t>
+              <a:t>Probability of finding a Productive Well based on</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> 3.70 </a:t>
+              <a:t> # of Drilled Holes</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -294,6 +294,66 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Y</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> (# of Holes drilled)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -358,6 +418,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>p(y)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -480,13 +595,8 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Problem</a:t>
+              <a:t>Probability of finding a person who prefers a toothpaste brand based on # of people interviewed</a:t>
             </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> 3.78</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -619,6 +729,61 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Y (# of people interviewed)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -683,6 +848,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>p(y)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -805,11 +1025,24 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Problem 3.43</a:t>
+              <a:t>Probability</a:t>
             </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> of finding people qualified for favorable rates</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.16111111111111112"/>
+          <c:y val="3.2407407407407406E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -909,6 +1142,61 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Y (# of people selected)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -974,6 +1262,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>p(y)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1088,12 +1431,8 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Problem</a:t>
-            </a:r>
-            <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> 3.45</a:t>
+              <a:t>Probability of activating the active alarm</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1191,6 +1530,66 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Y (#</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> of cells)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1256,6 +1655,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>p(y)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -3591,7 +4045,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>28</xdr:col>
-      <xdr:colOff>53340</xdr:colOff>
+      <xdr:colOff>350520</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>45720</xdr:rowOff>
     </xdr:to>
@@ -3627,7 +4081,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>28</xdr:col>
-      <xdr:colOff>22860</xdr:colOff>
+      <xdr:colOff>320040</xdr:colOff>
       <xdr:row>33</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
@@ -3976,8 +4430,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{690F194F-7AE2-4943-BC19-11D22EE53B20}">
   <dimension ref="A1:T36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T11" sqref="T11"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="AD30" sqref="AD30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>